<commit_message>
Finished Logical, probably, and mostly updated Physical (also turned it into an Excel file).
</commit_message>
<xml_diff>
--- a/Logical.xlsx
+++ b/Logical.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MTCStudent\Desktop\OnlineService\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="330" windowWidth="19740" windowHeight="7620"/>
   </bookViews>
@@ -16,12 +11,32 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="A10000000">Sheet1!$A$100000</definedName>
+    <definedName name="A1000000000">Sheet1!$A$100000</definedName>
+    <definedName name="A1050000">Sheet1!$A$1000020</definedName>
+    <definedName name="A1100000">Sheet1!$A$1000020</definedName>
+    <definedName name="A1500000">Sheet1!$A$1000020</definedName>
+    <definedName name="A1999999">Sheet1!$A$1000020</definedName>
+    <definedName name="A2000000">Sheet1!$A$1000000</definedName>
+    <definedName name="A5000000">Sheet1!$A$1000000</definedName>
+    <definedName name="A9999998">Sheet1!$A$1000000</definedName>
+    <definedName name="A9999999">Sheet1!$A$1000000</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>sam is stinky</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,22 +93,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="25" name="Group 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -101,7 +116,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3743325" y="4657725"/>
+          <a:off x="4095750" y="5353050"/>
           <a:ext cx="1733550" cy="742950"/>
           <a:chOff x="2466975" y="2143125"/>
           <a:chExt cx="1733550" cy="742950"/>
@@ -112,7 +127,7 @@
           <xdr:cNvPr id="11" name="Rectangle 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -158,7 +173,7 @@
           <xdr:cNvPr id="36" name="Rectangle 35">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -204,7 +219,7 @@
           <xdr:cNvPr id="37" name="Rectangle 36">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -250,23 +265,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="28" name="Group 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -274,7 +289,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1057275" y="4657725"/>
+          <a:off x="1828800" y="5314950"/>
           <a:ext cx="1733550" cy="990600"/>
           <a:chOff x="1647825" y="1809750"/>
           <a:chExt cx="1733550" cy="990600"/>
@@ -285,7 +300,7 @@
           <xdr:cNvPr id="39" name="Group 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -304,7 +319,7 @@
             <xdr:cNvPr id="40" name="Rectangle 39">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000028000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -350,7 +365,7 @@
             <xdr:cNvPr id="41" name="Rectangle 40">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -396,7 +411,7 @@
             <xdr:cNvPr id="42" name="Rectangle 41">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -443,7 +458,7 @@
           <xdr:cNvPr id="43" name="Rectangle 42">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -510,7 +525,7 @@
         <xdr:cNvPr id="29" name="Group 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -529,7 +544,7 @@
           <xdr:cNvPr id="45" name="Group 44">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -548,7 +563,7 @@
             <xdr:cNvPr id="46" name="Group 45">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -567,7 +582,7 @@
               <xdr:cNvPr id="48" name="Rectangle 47">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -613,7 +628,7 @@
               <xdr:cNvPr id="49" name="Rectangle 48">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000031000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -659,7 +674,7 @@
               <xdr:cNvPr id="50" name="Rectangle 49">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000032000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -706,7 +721,7 @@
             <xdr:cNvPr id="47" name="Rectangle 46">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -753,7 +768,7 @@
           <xdr:cNvPr id="57" name="Rectangle 56">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000039000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -799,23 +814,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="59" name="Group 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -823,7 +838,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6467475" y="657225"/>
+          <a:off x="142875" y="3790950"/>
           <a:ext cx="1733550" cy="1238250"/>
           <a:chOff x="314325" y="466725"/>
           <a:chExt cx="1733550" cy="1238250"/>
@@ -834,7 +849,7 @@
           <xdr:cNvPr id="60" name="Group 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -853,7 +868,7 @@
             <xdr:cNvPr id="62" name="Group 61">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -872,7 +887,7 @@
               <xdr:cNvPr id="64" name="Rectangle 63">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000040000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -926,7 +941,7 @@
               <xdr:cNvPr id="65" name="Rectangle 64">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000041000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -972,7 +987,7 @@
               <xdr:cNvPr id="66" name="Rectangle 65">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1019,7 +1034,7 @@
             <xdr:cNvPr id="63" name="Rectangle 62">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1071,7 +1086,7 @@
           <xdr:cNvPr id="61" name="Rectangle 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1133,7 +1148,7 @@
         <xdr:cNvPr id="67" name="Group 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000043000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1152,7 +1167,7 @@
           <xdr:cNvPr id="68" name="Rectangle 67">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000044000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1198,7 +1213,7 @@
           <xdr:cNvPr id="69" name="Rectangle 68">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1244,7 +1259,7 @@
           <xdr:cNvPr id="70" name="Rectangle 69">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000046000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1306,7 +1321,7 @@
         <xdr:cNvPr id="71" name="Group 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1325,7 +1340,7 @@
           <xdr:cNvPr id="72" name="Rectangle 71">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000048000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1371,7 +1386,7 @@
           <xdr:cNvPr id="73" name="Rectangle 72">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000049000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1433,7 +1448,7 @@
         <xdr:cNvPr id="75" name="Group 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1452,7 +1467,7 @@
           <xdr:cNvPr id="76" name="Rectangle 75">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1498,7 +1513,7 @@
           <xdr:cNvPr id="77" name="Rectangle 76">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1544,7 +1559,7 @@
           <xdr:cNvPr id="78" name="Rectangle 77">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1606,7 +1621,7 @@
         <xdr:cNvPr id="30" name="Group 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1625,7 +1640,7 @@
           <xdr:cNvPr id="79" name="Group 78">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1644,7 +1659,7 @@
             <xdr:cNvPr id="80" name="Group 79">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000050000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1663,7 +1678,7 @@
               <xdr:cNvPr id="82" name="Group 81">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000052000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1682,7 +1697,7 @@
                 <xdr:cNvPr id="84" name="Rectangle 83">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000054000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -1728,7 +1743,7 @@
                 <xdr:cNvPr id="85" name="Rectangle 84">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000055000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -1774,7 +1789,7 @@
                 <xdr:cNvPr id="86" name="Rectangle 85">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000056000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -1821,7 +1836,7 @@
               <xdr:cNvPr id="83" name="Rectangle 82">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1868,7 +1883,7 @@
             <xdr:cNvPr id="81" name="Rectangle 80">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000051000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1915,7 +1930,7 @@
           <xdr:cNvPr id="87" name="Rectangle 86">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000057000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1961,7 +1976,7 @@
           <xdr:cNvPr id="88" name="Rectangle 87">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000058000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2023,7 +2038,7 @@
         <xdr:cNvPr id="90" name="Group 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2042,7 +2057,7 @@
           <xdr:cNvPr id="91" name="Group 90">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2061,7 +2076,7 @@
             <xdr:cNvPr id="94" name="Group 93">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2080,7 +2095,7 @@
               <xdr:cNvPr id="96" name="Group 95">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000060000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2099,7 +2114,7 @@
                 <xdr:cNvPr id="98" name="Rectangle 97">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000062000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -2145,7 +2160,7 @@
                 <xdr:cNvPr id="99" name="Rectangle 98">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000063000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -2191,7 +2206,7 @@
                 <xdr:cNvPr id="100" name="Rectangle 99">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000064000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -2238,7 +2253,7 @@
               <xdr:cNvPr id="97" name="Rectangle 96">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000061000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2285,7 +2300,7 @@
             <xdr:cNvPr id="95" name="Rectangle 94">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2332,7 +2347,7 @@
           <xdr:cNvPr id="92" name="Rectangle 91">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2378,23 +2393,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="32" name="Straight Connector 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2405,8 +2420,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5476875" y="4924425"/>
-          <a:ext cx="1000125" cy="104775"/>
+          <a:off x="5829300" y="4924425"/>
+          <a:ext cx="647700" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2431,23 +2446,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="34" name="Straight Connector 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2458,8 +2473,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2790825" y="4781550"/>
-          <a:ext cx="952500" cy="0"/>
+          <a:off x="3562350" y="5438775"/>
+          <a:ext cx="533400" cy="38100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2500,7 +2515,7 @@
         <xdr:cNvPr id="38" name="Straight Connector 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2553,7 +2568,7 @@
         <xdr:cNvPr id="108" name="Group 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2572,7 +2587,7 @@
           <xdr:cNvPr id="109" name="Group 108">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2591,7 +2606,7 @@
             <xdr:cNvPr id="111" name="Group 110">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2610,7 +2625,7 @@
               <xdr:cNvPr id="113" name="Rectangle 112">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000071000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2656,7 +2671,7 @@
               <xdr:cNvPr id="114" name="Rectangle 113">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000072000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2707,7 +2722,7 @@
               <xdr:cNvPr id="115" name="Rectangle 114">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2754,7 +2769,7 @@
             <xdr:cNvPr id="112" name="Rectangle 111">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000070000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2801,7 +2816,7 @@
           <xdr:cNvPr id="110" name="Rectangle 109">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2863,7 +2878,7 @@
         <xdr:cNvPr id="101" name="Straight Connector 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2916,7 +2931,7 @@
         <xdr:cNvPr id="103" name="Straight Connector 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000067000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2969,7 +2984,7 @@
         <xdr:cNvPr id="105" name="Straight Connector 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3022,7 +3037,7 @@
         <xdr:cNvPr id="107" name="Straight Connector 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3075,7 +3090,7 @@
         <xdr:cNvPr id="117" name="Straight Connector 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000075000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3112,23 +3127,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="127" name="Group 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3136,7 +3151,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8772525" y="1114425"/>
+          <a:off x="1609725" y="1266825"/>
           <a:ext cx="1733550" cy="1238250"/>
           <a:chOff x="314325" y="466725"/>
           <a:chExt cx="1733550" cy="1238250"/>
@@ -3147,7 +3162,7 @@
           <xdr:cNvPr id="128" name="Group 127">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000080000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3166,7 +3181,7 @@
             <xdr:cNvPr id="130" name="Group 129">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000082000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3185,7 +3200,7 @@
               <xdr:cNvPr id="132" name="Rectangle 131">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000084000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3220,12 +3235,8 @@
               <a:p>
                 <a:pPr algn="ctr"/>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100" b="1"/>
-                  <a:t>Bank</a:t>
-                </a:r>
-                <a:r>
                   <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-                  <a:t> </a:t>
+                  <a:t>Other </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" b="1"/>
@@ -3239,7 +3250,7 @@
               <xdr:cNvPr id="133" name="Rectangle 132">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000085000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3285,7 +3296,7 @@
               <xdr:cNvPr id="134" name="Rectangle 133">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000086000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000086000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3332,7 +3343,7 @@
             <xdr:cNvPr id="131" name="Rectangle 130">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000083000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3368,13 +3379,8 @@
               <a:pPr algn="l"/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100"/>
-                <a:t>Card</a:t>
+                <a:t>Account Type</a:t>
               </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                <a:t> Number</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -3384,7 +3390,7 @@
           <xdr:cNvPr id="129" name="Rectangle 128">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000081000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3420,12 +3426,113 @@
             <a:pPr algn="l"/>
             <a:r>
               <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Card Expiration Date</a:t>
+              <a:t>Account</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> Holder</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Elbow Connector 8"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="61" idx="3"/>
+          <a:endCxn id="85" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1876425" y="4429125"/>
+          <a:ext cx="4600575" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Elbow Connector 18"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="129" idx="2"/>
+          <a:endCxn id="84" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3638550" y="1343025"/>
+          <a:ext cx="1676400" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3474,7 +3581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3507,26 +3614,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3559,23 +3649,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3752,16 +3825,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1048576" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated models to reflect current structure.
</commit_message>
<xml_diff>
--- a/Logical.xlsx
+++ b/Logical.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MTCStudent\Desktop\OnlineService\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="330" windowWidth="19740" windowHeight="7620"/>
   </bookViews>
@@ -28,15 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>sam is stinky</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,7 +109,7 @@
         <xdr:cNvPr id="25" name="Group 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -127,7 +128,7 @@
           <xdr:cNvPr id="11" name="Rectangle 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -173,7 +174,7 @@
           <xdr:cNvPr id="36" name="Rectangle 35">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -219,7 +220,7 @@
           <xdr:cNvPr id="37" name="Rectangle 36">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -281,7 +282,7 @@
         <xdr:cNvPr id="28" name="Group 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -300,7 +301,7 @@
           <xdr:cNvPr id="39" name="Group 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -319,7 +320,7 @@
             <xdr:cNvPr id="40" name="Rectangle 39">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -365,7 +366,7 @@
             <xdr:cNvPr id="41" name="Rectangle 40">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -411,7 +412,7 @@
             <xdr:cNvPr id="42" name="Rectangle 41">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -458,7 +459,7 @@
           <xdr:cNvPr id="43" name="Rectangle 42">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -525,7 +526,7 @@
         <xdr:cNvPr id="29" name="Group 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -544,7 +545,7 @@
           <xdr:cNvPr id="45" name="Group 44">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -563,7 +564,7 @@
             <xdr:cNvPr id="46" name="Group 45">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -582,7 +583,7 @@
               <xdr:cNvPr id="48" name="Rectangle 47">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -628,7 +629,7 @@
               <xdr:cNvPr id="49" name="Rectangle 48">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -674,7 +675,7 @@
               <xdr:cNvPr id="50" name="Rectangle 49">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -721,7 +722,7 @@
             <xdr:cNvPr id="47" name="Rectangle 46">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -768,7 +769,7 @@
           <xdr:cNvPr id="57" name="Rectangle 56">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -830,7 +831,7 @@
         <xdr:cNvPr id="59" name="Group 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -849,7 +850,7 @@
           <xdr:cNvPr id="60" name="Group 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -868,7 +869,7 @@
             <xdr:cNvPr id="62" name="Group 61">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -887,7 +888,7 @@
               <xdr:cNvPr id="64" name="Rectangle 63">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -941,7 +942,7 @@
               <xdr:cNvPr id="65" name="Rectangle 64">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -987,7 +988,7 @@
               <xdr:cNvPr id="66" name="Rectangle 65">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1034,7 +1035,7 @@
             <xdr:cNvPr id="63" name="Rectangle 62">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1086,7 +1087,7 @@
           <xdr:cNvPr id="61" name="Rectangle 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1148,7 +1149,7 @@
         <xdr:cNvPr id="67" name="Group 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1167,7 +1168,7 @@
           <xdr:cNvPr id="68" name="Rectangle 67">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1213,7 +1214,7 @@
           <xdr:cNvPr id="69" name="Rectangle 68">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1259,7 +1260,7 @@
           <xdr:cNvPr id="70" name="Rectangle 69">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1321,7 +1322,7 @@
         <xdr:cNvPr id="71" name="Group 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1340,7 +1341,7 @@
           <xdr:cNvPr id="72" name="Rectangle 71">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1386,7 +1387,7 @@
           <xdr:cNvPr id="73" name="Rectangle 72">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1448,7 +1449,7 @@
         <xdr:cNvPr id="75" name="Group 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,7 +1468,7 @@
           <xdr:cNvPr id="76" name="Rectangle 75">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1513,7 +1514,7 @@
           <xdr:cNvPr id="77" name="Rectangle 76">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1559,7 +1560,7 @@
           <xdr:cNvPr id="78" name="Rectangle 77">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1621,7 +1622,7 @@
         <xdr:cNvPr id="90" name="Group 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1640,7 +1641,7 @@
           <xdr:cNvPr id="91" name="Group 90">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1659,7 +1660,7 @@
             <xdr:cNvPr id="94" name="Group 93">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1678,7 +1679,7 @@
               <xdr:cNvPr id="96" name="Group 95">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1697,7 +1698,7 @@
                 <xdr:cNvPr id="98" name="Rectangle 97">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -1743,7 +1744,7 @@
                 <xdr:cNvPr id="99" name="Rectangle 98">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -1789,7 +1790,7 @@
                 <xdr:cNvPr id="100" name="Rectangle 99">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -1836,7 +1837,7 @@
               <xdr:cNvPr id="97" name="Rectangle 96">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1883,7 +1884,7 @@
             <xdr:cNvPr id="95" name="Rectangle 94">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1930,7 +1931,7 @@
           <xdr:cNvPr id="92" name="Rectangle 91">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1992,7 +1993,7 @@
         <xdr:cNvPr id="32" name="Straight Connector 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2045,7 +2046,7 @@
         <xdr:cNvPr id="34" name="Straight Connector 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2098,7 +2099,7 @@
         <xdr:cNvPr id="38" name="Straight Connector 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2151,7 +2152,7 @@
         <xdr:cNvPr id="108" name="Group 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2170,7 +2171,7 @@
           <xdr:cNvPr id="109" name="Group 108">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2189,7 +2190,7 @@
             <xdr:cNvPr id="111" name="Group 110">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2208,7 +2209,7 @@
               <xdr:cNvPr id="113" name="Rectangle 112">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2254,7 +2255,7 @@
               <xdr:cNvPr id="114" name="Rectangle 113">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2305,7 +2306,7 @@
               <xdr:cNvPr id="115" name="Rectangle 114">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2352,7 +2353,7 @@
             <xdr:cNvPr id="112" name="Rectangle 111">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2399,7 +2400,7 @@
           <xdr:cNvPr id="110" name="Rectangle 109">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2461,7 +2462,7 @@
         <xdr:cNvPr id="103" name="Straight Connector 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2514,7 +2515,7 @@
         <xdr:cNvPr id="105" name="Straight Connector 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2567,7 +2568,7 @@
         <xdr:cNvPr id="107" name="Straight Connector 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2620,7 +2621,7 @@
         <xdr:cNvPr id="117" name="Straight Connector 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2673,7 +2674,7 @@
         <xdr:cNvPr id="127" name="Group 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2693,7 @@
           <xdr:cNvPr id="128" name="Group 127">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2711,7 +2712,7 @@
             <xdr:cNvPr id="130" name="Group 129">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2730,7 +2731,7 @@
               <xdr:cNvPr id="132" name="Rectangle 131">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2780,7 +2781,7 @@
               <xdr:cNvPr id="133" name="Rectangle 132">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2826,7 +2827,7 @@
               <xdr:cNvPr id="134" name="Rectangle 133">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000086000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000086000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2873,7 +2874,7 @@
             <xdr:cNvPr id="131" name="Rectangle 130">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2920,7 +2921,7 @@
           <xdr:cNvPr id="129" name="Rectangle 128">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2984,7 +2985,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Elbow Connector 8"/>
+        <xdr:cNvPr id="9" name="Elbow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="61" idx="3"/>
           <a:endCxn id="85" idx="1"/>
@@ -3033,7 +3040,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Elbow Connector 18"/>
+        <xdr:cNvPr id="19" name="Elbow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="129" idx="2"/>
           <a:endCxn id="84" idx="1"/>
@@ -3080,7 +3093,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="115" idx="1"/>
           <a:endCxn id="50" idx="3"/>
@@ -3127,7 +3146,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="115" idx="1"/>
           <a:endCxn id="64" idx="3"/>
@@ -3174,7 +3199,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:endCxn id="129" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -3220,7 +3251,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -3236,7 +3273,7 @@
           <xdr:cNvPr id="30" name="Group 29">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3255,7 +3292,7 @@
             <xdr:cNvPr id="79" name="Group 78">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3274,7 +3311,7 @@
               <xdr:cNvPr id="80" name="Group 79">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3293,7 +3330,7 @@
                 <xdr:cNvPr id="82" name="Group 81">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -3312,7 +3349,7 @@
                   <xdr:cNvPr id="84" name="Rectangle 83">
                     <a:extLst>
                       <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                        <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054000000}"/>
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054000000}"/>
                       </a:ext>
                     </a:extLst>
                   </xdr:cNvPr>
@@ -3358,7 +3395,7 @@
                   <xdr:cNvPr id="85" name="Rectangle 84">
                     <a:extLst>
                       <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                        <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
                       </a:ext>
                     </a:extLst>
                   </xdr:cNvPr>
@@ -3404,7 +3441,7 @@
                   <xdr:cNvPr id="86" name="Rectangle 85">
                     <a:extLst>
                       <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                        <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
                       </a:ext>
                     </a:extLst>
                   </xdr:cNvPr>
@@ -3451,7 +3488,7 @@
                 <xdr:cNvPr id="83" name="Rectangle 82">
                   <a:extLst>
                     <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
                     </a:ext>
                   </a:extLst>
                 </xdr:cNvPr>
@@ -3498,7 +3535,7 @@
               <xdr:cNvPr id="81" name="Rectangle 80">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3545,7 +3582,7 @@
             <xdr:cNvPr id="87" name="Rectangle 86">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3591,7 +3628,7 @@
             <xdr:cNvPr id="88" name="Rectangle 87">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3638,7 +3675,7 @@
           <xdr:cNvPr id="93" name="Rectangle 92">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3687,6 +3724,769 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="106" name="Group 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CF83560-6AC5-43F3-9748-28BE1F64DD58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9067800" y="6686550"/>
+          <a:ext cx="1733550" cy="990600"/>
+          <a:chOff x="1647825" y="1809750"/>
+          <a:chExt cx="1733550" cy="990600"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="118" name="Group 117">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F38D7DD5-31DA-4F93-B3BD-44DF59064724}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1647825" y="1809750"/>
+            <a:ext cx="1733550" cy="742950"/>
+            <a:chOff x="2466975" y="2143125"/>
+            <a:chExt cx="1733550" cy="742950"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="120" name="Rectangle 119">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A9FC58E-16D0-4001-92FB-F7A40E4D47C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2466975" y="2143125"/>
+              <a:ext cx="1733550" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1"/>
+                <a:t>Member Login</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="121" name="Rectangle 120">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D2D9DB-BA02-4339-9A82-C773BF2760A2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2466975" y="2390775"/>
+              <a:ext cx="1733550" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Member</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="122" name="Rectangle 121">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B16B3A-107A-4449-A362-2D2011A69AF3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2466975" y="2638425"/>
+              <a:ext cx="1733550" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Member</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> Login</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="119" name="Rectangle 118">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4900794-BCF6-4606-8FE7-0C7B520D2CE4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1647825" y="2552700"/>
+            <a:ext cx="1733550" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Password</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="126" name="Group 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5325F88-BFF8-4093-B29D-0E4EAB886CE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9201150" y="1666875"/>
+          <a:ext cx="1733550" cy="742950"/>
+          <a:chOff x="2466975" y="2143125"/>
+          <a:chExt cx="1733550" cy="742950"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="136" name="Rectangle 135">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0D6CBD5-A71F-4B9E-8B20-55C05670B6D0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2466975" y="2143125"/>
+            <a:ext cx="1733550" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Member Email</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="137" name="Rectangle 136">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA00684-407C-4A3C-BD90-5DEA3FCBC5B6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2466975" y="2390775"/>
+            <a:ext cx="1733550" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Member</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="138" name="Rectangle 137">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{828BE728-B426-4F25-9D9C-098BCA652672}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2466975" y="2638425"/>
+            <a:ext cx="1733550" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Email</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connector: Elbow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4952FB62-78AF-46C9-B16F-7725FED465E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="85" idx="3"/>
+          <a:endCxn id="137" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8210550" y="2038350"/>
+          <a:ext cx="990600" cy="2390775"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="140" name="Group 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2507CB49-70F8-4DD5-B675-5ABD6C6C2408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9191625" y="314325"/>
+          <a:ext cx="1733550" cy="990600"/>
+          <a:chOff x="1647825" y="1809750"/>
+          <a:chExt cx="1733550" cy="990600"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="142" name="Group 141">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB7F63C-9606-499A-8ABD-94FCA20A7A77}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1647825" y="1809750"/>
+            <a:ext cx="1733550" cy="742950"/>
+            <a:chOff x="2466975" y="2143125"/>
+            <a:chExt cx="1733550" cy="742950"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="144" name="Rectangle 143">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18078AA0-4C14-46FF-9DF6-FAA389F02085}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2466975" y="2143125"/>
+              <a:ext cx="1733550" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+                <a:t>Member Phone</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="145" name="Rectangle 144">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A88CF59F-9903-491E-8958-745A88D021F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2466975" y="2390775"/>
+              <a:ext cx="1733550" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Member</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="146" name="Rectangle 145">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EBD1323-452C-4F3E-8735-0F7116F8A120}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2466975" y="2638425"/>
+              <a:ext cx="1733550" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Phone Number</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="143" name="Rectangle 142">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC5C395-B481-4BB8-8A5D-6A369A36395E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1647825" y="2552700"/>
+            <a:ext cx="1733550" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Type of Phone</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connector: Elbow 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6A0C6D-94C4-4C29-B63C-12D9AF2D5E58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="146" idx="1"/>
+          <a:endCxn id="84" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="8210551" y="933449"/>
+          <a:ext cx="981075" cy="3248025"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3733,7 +4533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3766,9 +4566,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3801,6 +4618,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3977,21 +4811,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1048576"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-    </row>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1048576" t="s">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>